<commit_message>
Adjusted stuff in Meilenstein I folder to meet the requirements (available in pdf) as well as adding README.txt
</commit_message>
<xml_diff>
--- a/Meilenstein I/Protocol Draft.xlsx
+++ b/Meilenstein I/Protocol Draft.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Desktop\PROGRAMMIERPROJEKT\Gruppe-8\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Desktop\PROGRAMMIERPROJEKT\Gruppe-8\Meilenstein I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF091A56-F5A9-4BC1-A42F-9F4BCCA78FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD06589-F77F-4AB9-833D-EC67EE500E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="983" yWindow="-98" windowWidth="21614" windowHeight="15196" xr2:uid="{E8FC162F-0F97-48EB-9F5D-6FC7A7A87B98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>CLIENT message</t>
   </si>
@@ -155,6 +155,9 @@
       </rPr>
       <t>: send ghost / not ghost status to everyone</t>
     </r>
+  </si>
+  <si>
+    <t>This is a rough demo of the client / server protocol.</t>
   </si>
 </sst>
 </file>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE273F8A-FF89-47E0-9630-7DDE1F2CB04A}">
-  <dimension ref="B1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="105" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -583,145 +586,150 @@
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+    <row r="4" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+    <row r="7" spans="1:4" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="41.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="41.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:4" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="71.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="71.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="16" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:4" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>